<commit_message>
Dev Computer 16/05/2023 01
</commit_message>
<xml_diff>
--- a/production_public/assets/v2/samples/new_excel_registration.xlsx
+++ b/production_public/assets/v2/samples/new_excel_registration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srvro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\htdocs\AMG\plus_db\client_dashboards\version_one\plus_database\production_public\assets\v2\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D3D96-AFA2-427B-AC3E-1AD1E2336534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFB0A73-6939-4DFB-B816-4DE0540C45AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="1170" windowWidth="20505" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1170" windowWidth="20505" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>0209075691</t>
   </si>
   <si>
-    <t>Registered Member</t>
-  </si>
-  <si>
     <t>Main Branch</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>0002</t>
+  </si>
+  <si>
+    <t>Membership</t>
   </si>
 </sst>
 </file>
@@ -191,6 +191,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -533,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -638,16 +639,16 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>11</v>
@@ -668,7 +669,7 @@
         <v>14</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -691,16 +692,16 @@
         <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>13</v>
@@ -715,7 +716,7 @@
         <v>21</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>